<commit_message>
fix to VW parts display
</commit_message>
<xml_diff>
--- a/config/vw_parts.xlsx
+++ b/config/vw_parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6418f5b8b750208/Code/356_parts/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1168" documentId="8_{08365CD5-F318-9946-A7DC-86CF9963F12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCE1F637-A315-FD4D-AA42-0FBE3A4BB9A4}"/>
+  <xr:revisionPtr revIDLastSave="1205" documentId="8_{08365CD5-F318-9946-A7DC-86CF9963F12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F27517B-E9C1-8C41-AE3B-C9C38E22C25D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="21000" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group3-4" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>part-no</t>
   </si>
@@ -101,15 +101,6 @@
     <t>10B</t>
   </si>
   <si>
-    <t>311511245, 311511246</t>
-  </si>
-  <si>
-    <t>Outer spring plate busging left &amp; right side</t>
-  </si>
-  <si>
-    <t>1 ea</t>
-  </si>
-  <si>
     <t>each bushing specific to side</t>
   </si>
   <si>
@@ -138,13 +129,49 @@
   </si>
   <si>
     <t>https://www.skf.com/id/productinfo/productid-6306%2FC3</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>111511245E.jpg</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>311511246</t>
+  </si>
+  <si>
+    <t>311511246.jpg</t>
+  </si>
+  <si>
+    <t>311511245</t>
+  </si>
+  <si>
+    <t>311511245.jpg</t>
+  </si>
+  <si>
+    <t>Outer spring plate bushing left side</t>
+  </si>
+  <si>
+    <t>Outer spring plate busging right side</t>
+  </si>
+  <si>
+    <t>111498051.jpg</t>
+  </si>
+  <si>
+    <t>111498021.jpg</t>
+  </si>
+  <si>
+    <t>6306.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,11 +183,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -177,16 +199,47 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -194,34 +247,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -243,171 +331,60 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -422,27 +399,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I4" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I4">
-    <sortCondition ref="E1:E4"/>
-  </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="diagram_name" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{26B54F8E-BF5D-8F46-84D4-AD3810497338}" name="ref" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="website" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="group" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="item" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="description" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="part-no" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="qty" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{E2BFE521-0ABD-424B-9159-1CAF84470C53}" name="Notes" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -766,108 +722,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8419CACA-44BF-1546-811D-F9987A0E7488}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="13"/>
-    <col min="3" max="3" width="29" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="27.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="14"/>
-    <col min="9" max="9" width="43.1640625" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="13"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="10.83203125" style="8"/>
+    <col min="3" max="3" width="29" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="8"/>
+    <col min="6" max="6" width="27.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="8"/>
+    <col min="10" max="10" width="43.1640625" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -886,156 +852,200 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" style="8" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="27.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="5"/>
-    <col min="9" max="9" width="42.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="63.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H4" s="22">
+        <v>2</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
+    <row r="5" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H5" s="27">
         <v>2</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I5" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="31" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:B8">
-    <sortCondition ref="B5:B8"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:B9">
+    <sortCondition ref="B6:B9"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{1DAEA6EA-6D0F-1B49-989D-7AD09364FD21}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{33F0B994-29C9-6241-87DC-46D769385306}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{8D5A9504-0A0D-4F49-9CEA-F89E150F49A7}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{33F0B994-29C9-6241-87DC-46D769385306}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{8D5A9504-0A0D-4F49-9CEA-F89E150F49A7}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{F36C51A9-75E0-9046-931B-E474B6868862}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId4"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>